<commit_message>
small update in tracker
</commit_message>
<xml_diff>
--- a/Track/MyTracker.xlsx
+++ b/Track/MyTracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="In Hand" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Mentor Graphics</t>
   </si>
@@ -242,12 +242,28 @@
     <t>On carre site of MicroFocus workday
 hrudwik@gmail.com</t>
   </si>
+  <si>
+    <t>Salesforce</t>
+  </si>
+  <si>
+    <t>Tricentis</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>1. Contacted by recruiter  
+"Mayuri Girdhar"</t>
+  </si>
+  <si>
+    <t>Contacted on 2nd Jan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +285,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Garamond"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -303,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -345,6 +368,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,53 +750,53 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -776,10 +805,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,150 +871,199 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
-        <v>3</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B9" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>2</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>